<commit_message>
adjustments for SA and simu
</commit_message>
<xml_diff>
--- a/simulations/inputs/Factorial_plan_SA.xlsx
+++ b/simulations/inputs/Factorial_plan_SA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\sshfs\torisuten@192.168.12.9\pp\Wheat-BRIDGES\Root_BRIDGES\simulations\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B926737-92BE-40F8-B60E-A3AD9286E795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B00B50-3BFD-40E9-9225-4BD6E6FC5FF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1156,15 +1156,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="11" fontId="16" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="16" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1175,13 +1174,13 @@
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1509,7 +1508,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1527,204 +1526,204 @@
       <c r="A1" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="10" t="s">
         <v>200</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="4">
         <v>1E-3</v>
       </c>
-      <c r="F2" s="5">
-        <v>5.0000000000000001E-4</v>
-      </c>
-      <c r="G2" s="5">
+      <c r="F2" s="4">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="G2" s="4">
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>29</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="4">
         <v>25</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="4">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+    <row r="4" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="10" t="s">
         <v>202</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>150</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>150</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="4">
         <v>300</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="4" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+    <row r="5" spans="1:7" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>190</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>2.0833333333333335E-4</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>2.0833333333333335E-4</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="4">
         <v>2.0833333333333298E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>190</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>1.2500000000000001E-6</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>1.2500000000000001E-6</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="4">
         <v>2.5000000000000001E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="5">
+      <c r="D7" s="10"/>
+      <c r="E7" s="4">
         <v>4.9999999999999995E-11</v>
       </c>
-      <c r="F7" s="5">
-        <v>4.9999999999999995E-11</v>
-      </c>
-      <c r="G7" s="5">
+      <c r="F7" s="4">
         <v>4.9999999999999997E-12</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="G7" s="4">
+        <v>5.0000000000000002E-11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
         <v>191</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="10" t="s">
         <v>193</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="10" t="s">
         <v>192</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="10" t="s">
         <v>196</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <v>9.9999999999999994E-12</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <v>5.9999999999999997E-13</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="4">
         <v>9.9999999999999994E-12</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
         <v>194</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="10" t="s">
         <v>195</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="10" t="s">
         <v>190</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="4">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <v>1E-4</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="4">
         <v>1E-3</v>
       </c>
     </row>

</xml_diff>